<commit_message>
Add Diary, Find FlashLight in Box MiniGame
</commit_message>
<xml_diff>
--- a/Assets/Editor/JsonUtility/JsonUtility/Stage1/Small Room.xlsx
+++ b/Assets/Editor/JsonUtility/JsonUtility/Stage1/Small Room.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UISU\Documents\GitHub\Project_Caterpillar\Assets\Editor\JsonUtility\JsonUtility\Stage1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/uisoo/Documents/GitHub/Project-Caterpillar/Assets/Editor/JsonUtility/JsonUtility/Stage1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CEAE2E-1DB5-4D20-BF82-8171E452F70B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{628ACFD1-02AC-0E44-9CA2-E937EA1FB414}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="!Sample" sheetId="1" r:id="rId1"/>
@@ -1421,7 +1421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="139">
   <si>
     <t>파일명</t>
   </si>
@@ -1987,6 +1987,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2367,9 +2368,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="26" width="8.85546875" customWidth="1"/>
+    <col min="1" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -3447,14 +3448,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -4576,14 +4577,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -5707,19 +5708,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="72.5703125" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="72.5" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="59.7109375" customWidth="1"/>
-    <col min="7" max="26" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="59.6640625" customWidth="1"/>
+    <col min="7" max="26" width="8.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" ht="16.5" customHeight="1">
@@ -7486,17 +7487,17 @@
   <dimension ref="A1:F1003"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="D13" sqref="D13:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.85546875" customWidth="1"/>
-    <col min="2" max="2" width="78.85546875" customWidth="1"/>
+    <col min="1" max="1" width="10.83203125" customWidth="1"/>
+    <col min="2" max="2" width="78.83203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -7688,9 +7689,13 @@
       <c r="C13" s="8">
         <v>1</v>
       </c>
-      <c r="D13" s="8"/>
+      <c r="D13" s="8">
+        <v>4</v>
+      </c>
       <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
+      <c r="F13" s="8" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="14" spans="1:6" ht="16.5" customHeight="1">
       <c r="A14" s="8" t="s">
@@ -8967,11 +8972,11 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -10071,17 +10076,17 @@
   <dimension ref="A1:F1002"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="77.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="77.5" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -10232,6 +10237,12 @@
       </c>
       <c r="C11" s="1">
         <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="16.5" customHeight="1">
@@ -11246,14 +11257,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" customWidth="1"/>
+    <col min="2" max="2" width="46.5" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -12359,14 +12370,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -13472,14 +13483,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">
@@ -14595,14 +14606,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
-    <col min="2" max="2" width="74.28515625" customWidth="1"/>
+    <col min="2" max="2" width="74.33203125" customWidth="1"/>
     <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" customWidth="1"/>
-    <col min="7" max="26" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="9.5" customWidth="1"/>
+    <col min="7" max="26" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="16.5" customHeight="1">

</xml_diff>